<commit_message>
fix JobDescription convertion datetime from string
</commit_message>
<xml_diff>
--- a/Tracker.xlsx
+++ b/Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Evgeniy/Sources/async-python-sprint-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44216E5-BF68-084A-9B33-68004BD29296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA507827-E0F1-B24C-BEA2-14A8402FABDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16080" xr2:uid="{BD96139B-9345-3446-9F54-C741680B3838}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t xml:space="preserve"> Добавить TASK создающие файл (любой)</t>
   </si>
@@ -123,6 +123,12 @@
   </si>
   <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>SC-11</t>
+  </si>
+  <si>
+    <t>Добавть юнит-тесты для JobDescription маппинга из JSON</t>
   </si>
 </sst>
 </file>
@@ -527,15 +533,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C628440-54D5-614F-96E4-F1E8F32AEADE}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -557,46 +563,46 @@
     </row>
     <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
         <v>21</v>
       </c>
+      <c r="E3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" t="s">
         <v>27</v>
@@ -604,10 +610,10 @@
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6" t="s">
         <v>27</v>
@@ -615,21 +621,21 @@
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" t="s">
         <v>26</v>
@@ -637,10 +643,10 @@
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
         <v>26</v>
@@ -648,10 +654,10 @@
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="D10" t="s">
         <v>26</v>
@@ -659,18 +665,29 @@
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="D11" t="s">
         <v>26</v>
       </c>
     </row>
+    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E11">
-    <sortCondition ref="D2:D11"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E12">
+    <sortCondition ref="D2:D12"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add new tracker tasks
</commit_message>
<xml_diff>
--- a/Tracker.xlsx
+++ b/Tracker.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Evgeniy/Sources/async-python-sprint-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA507827-E0F1-B24C-BEA2-14A8402FABDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CE3CC8-678C-F740-B7CF-0CBBD5A0BCAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16080" xr2:uid="{BD96139B-9345-3446-9F54-C741680B3838}"/>
+    <workbookView xWindow="920" yWindow="2180" windowWidth="28040" windowHeight="16080" xr2:uid="{BD96139B-9345-3446-9F54-C741680B3838}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$15</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
   <si>
     <t xml:space="preserve"> Добавить TASK создающие файл (любой)</t>
   </si>
@@ -59,9 +62,6 @@
     <t xml:space="preserve"> параметризация ТАСК</t>
   </si>
   <si>
-    <t xml:space="preserve"> Не работает зависимости</t>
-  </si>
-  <si>
     <t>Task</t>
   </si>
   <si>
@@ -128,7 +128,40 @@
     <t>SC-11</t>
   </si>
   <si>
-    <t>Добавть юнит-тесты для JobDescription маппинга из JSON</t>
+    <t>SC-12</t>
+  </si>
+  <si>
+    <t>Файл не создается если нет директории (путь указан не верно)</t>
+  </si>
+  <si>
+    <t>Добавить юнит-тесты для JobDescription маппинга из JSON</t>
+  </si>
+  <si>
+    <t>SC-13</t>
+  </si>
+  <si>
+    <t>Конвертация datetime в строку и обратно</t>
+  </si>
+  <si>
+    <t>SC-14</t>
+  </si>
+  <si>
+    <t>Разработать класс конфигурации</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Не работают зависимости</t>
+  </si>
+  <si>
+    <t>SC-15</t>
+  </si>
+  <si>
+    <t>Логиррование</t>
+  </si>
+  <si>
+    <t>SC-16</t>
+  </si>
+  <si>
+    <t>Добавить аннотации</t>
   </si>
 </sst>
 </file>
@@ -533,159 +566,232 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C628440-54D5-614F-96E4-F1E8F32AEADE}">
-  <dimension ref="A1:E12"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="51.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
         <v>25</v>
-      </c>
-      <c r="D9" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
         <v>26</v>
       </c>
     </row>
+    <row r="14" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="17" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:E15" xr:uid="{1C628440-54D5-614F-96E4-F1E8F32AEADE}">
+    <filterColumn colId="4">
+      <customFilters>
+        <customFilter operator="notEqual" val="done"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E12">
     <sortCondition ref="D2:D12"/>
   </sortState>

</xml_diff>